<commit_message>
2006 Monthly Time Charts
</commit_message>
<xml_diff>
--- a/2006/aggravated-assault-2006.xlsx
+++ b/2006/aggravated-assault-2006.xlsx
@@ -4,9 +4,10 @@
   <workbookPr/>
   <sheets>
     <sheet sheetId="1" name="victim-by-age-gender-and-race" state="visible" r:id="rId3"/>
-    <sheet sheetId="2" name="offender-by-age-gender-and-race" state="visible" r:id="rId4"/>
-    <sheet sheetId="3" name="relationship-of-victim-to-offen" state="visible" r:id="rId5"/>
-    <sheet sheetId="4" name="circumstances" state="visible" r:id="rId6"/>
+    <sheet sheetId="2" name="monthly-time-chart" state="visible" r:id="rId4"/>
+    <sheet sheetId="3" name="offender-by-age-gender-and-race" state="visible" r:id="rId5"/>
+    <sheet sheetId="4" name="relationship-of-victim-to-offen" state="visible" r:id="rId6"/>
+    <sheet sheetId="5" name="circumstances" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -64,9 +65,51 @@
     <t>Total</t>
   </si>
   <si>
+    <t>Month</t>
+  </si>
+  <si>
     <t>Offender Age, Gender and Race</t>
   </si>
   <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Number of Aggravated Assaults</t>
+  </si>
+  <si>
     <t>Race</t>
   </si>
   <si>
@@ -79,9 +122,18 @@
     <t>0-17</t>
   </si>
   <si>
+    <t>Relationship of Victim to Offender</t>
+  </si>
+  <si>
     <t>18-35</t>
   </si>
   <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Spouse</t>
+  </si>
+  <si>
     <t>36+</t>
   </si>
   <si>
@@ -97,61 +149,52 @@
     <t>White</t>
   </si>
   <si>
+    <t>Common-Law Spouse</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Sibling</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
     <t>Black</t>
   </si>
   <si>
+    <t>Grandparent</t>
+  </si>
+  <si>
+    <t>Grandchild</t>
+  </si>
+  <si>
     <t>American Indian/Alaskan Native</t>
   </si>
   <si>
+    <t>In-Law</t>
+  </si>
+  <si>
     <t>Asian/Pacific Islander</t>
   </si>
   <si>
+    <t>Stepparent</t>
+  </si>
+  <si>
+    <t>Stepchild</t>
+  </si>
+  <si>
     <t>Unknown</t>
   </si>
   <si>
+    <t>Stepsibling</t>
+  </si>
+  <si>
+    <t>Other Family Member</t>
+  </si>
+  <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Relationship of Victim to Offender</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Spouse</t>
-  </si>
-  <si>
-    <t>Common-Law Spouse</t>
-  </si>
-  <si>
-    <t>Parent</t>
-  </si>
-  <si>
-    <t>Sibling</t>
-  </si>
-  <si>
-    <t>Child</t>
-  </si>
-  <si>
-    <t>Grandparent</t>
-  </si>
-  <si>
-    <t>Grandchild</t>
-  </si>
-  <si>
-    <t>In-Law</t>
-  </si>
-  <si>
-    <t>Stepparent</t>
-  </si>
-  <si>
-    <t>Stepchild</t>
-  </si>
-  <si>
-    <t>Stepsibling</t>
-  </si>
-  <si>
-    <t>Other Family Member</t>
   </si>
   <si>
     <t>Victim Was Offender</t>
@@ -289,19 +332,23 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -311,10 +358,336 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" customWidth="1" max="1" width="53.71"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c t="s" s="1" r="A1">
-        <v>0</v>
+      <c t="s" s="4" r="A1">
+        <v>35</v>
+      </c>
+      <c t="s" s="4" r="B1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="4" r="A2">
+        <v>38</v>
+      </c>
+      <c s="4" r="B2">
+        <v>509.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="4" r="A3">
+        <v>44</v>
+      </c>
+      <c s="4" r="B3">
+        <v>34.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="4" r="A4">
+        <v>45</v>
+      </c>
+      <c s="4" r="B4">
+        <v>169.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="4" r="A5">
+        <v>46</v>
+      </c>
+      <c s="4" r="B5">
+        <v>261.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="4" r="A6">
+        <v>47</v>
+      </c>
+      <c s="4" r="B6">
+        <v>249.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c t="s" s="4" r="A7">
+        <v>49</v>
+      </c>
+      <c s="4" r="B7">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c t="s" s="4" r="A8">
+        <v>50</v>
+      </c>
+      <c s="4" r="B8">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" s="4" r="A9">
+        <v>52</v>
+      </c>
+      <c s="4" r="B9">
+        <v>67.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" s="4" r="A10">
+        <v>54</v>
+      </c>
+      <c s="4" r="B10">
+        <v>29.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" s="4" r="A11">
+        <v>55</v>
+      </c>
+      <c s="4" r="B11">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" s="4" r="A12">
+        <v>57</v>
+      </c>
+      <c s="4" r="B12">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="4" r="A13">
+        <v>58</v>
+      </c>
+      <c s="4" r="B13">
+        <v>223.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" s="4" r="A14">
+        <v>60</v>
+      </c>
+      <c s="4" r="B14">
+        <v>473.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" s="4" r="A15">
+        <v>61</v>
+      </c>
+      <c s="4" r="B15">
+        <v>2862.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c t="s" s="4" r="A16">
+        <v>62</v>
+      </c>
+      <c s="4" r="B16">
+        <v>437.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" s="4" r="A17">
+        <v>63</v>
+      </c>
+      <c s="4" r="B17">
+        <v>144.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="4" r="A18">
+        <v>64</v>
+      </c>
+      <c s="4" r="B18">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="4" r="A19">
+        <v>65</v>
+      </c>
+      <c s="4" r="B19">
+        <v>1093.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="4" r="A20">
+        <v>66</v>
+      </c>
+      <c s="4" r="B20">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="4" r="A21">
+        <v>67</v>
+      </c>
+      <c s="4" r="B21">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" s="4" r="A22">
+        <v>68</v>
+      </c>
+      <c s="4" r="B22">
+        <v>31.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" s="4" r="A23">
+        <v>69</v>
+      </c>
+      <c s="4" r="B23">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" s="4" r="A24">
+        <v>70</v>
+      </c>
+      <c s="4" r="B24">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" s="4" r="A25">
+        <v>71</v>
+      </c>
+      <c s="4" r="B25">
+        <v>1176.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c t="s" s="4" r="A26">
+        <v>72</v>
+      </c>
+      <c s="4" r="B26">
+        <v>3984.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c t="s" s="4" r="A27">
+        <v>73</v>
+      </c>
+      <c s="4" r="B27">
+        <v>2865.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" customWidth="1" max="1" width="35.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="4" r="A1">
+        <v>74</v>
+      </c>
+      <c t="s" s="4" r="B1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="4" r="A2">
+        <v>76</v>
+      </c>
+      <c s="4" r="B2">
+        <v>4378.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="4" r="A3">
+        <v>77</v>
+      </c>
+      <c s="4" r="B3">
+        <v>680.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="4" r="A4">
+        <v>78</v>
+      </c>
+      <c s="4" r="B4">
+        <v>59.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="4" r="A5">
+        <v>79</v>
+      </c>
+      <c s="4" r="B5">
+        <v>43.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="4" r="A6">
+        <v>80</v>
+      </c>
+      <c s="4" r="B6">
+        <v>67.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c t="s" s="4" r="A7">
+        <v>81</v>
+      </c>
+      <c s="4" r="B7">
+        <v>397.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c t="s" s="4" r="A8">
+        <v>82</v>
+      </c>
+      <c s="4" r="B8">
+        <v>108.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" s="4" r="A9">
+        <v>83</v>
+      </c>
+      <c s="4" r="B9">
+        <v>2328.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" s="4" r="A10">
+        <v>84</v>
+      </c>
+      <c s="4" r="B10">
+        <v>3701.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="3" r="A1">
+        <v>17</v>
       </c>
       <c s="1" r="H1"/>
       <c s="1" r="I1"/>
@@ -338,96 +711,96 @@
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c t="s" s="1" r="E2">
-        <v>3</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="B3">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c t="s" s="1" r="D3">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c t="s" s="1" r="E3">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c t="s" s="1" r="F3">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c t="s" s="1" r="G3">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c s="2" r="B4">
-        <v>638.0</v>
+        <v>718.0</v>
       </c>
       <c s="2" r="C4">
-        <v>2252.0</v>
+        <v>2241.0</v>
       </c>
       <c s="2" r="D4">
-        <v>1266.0</v>
+        <v>1070.0</v>
       </c>
       <c s="2" r="E4">
-        <v>297.0</v>
+        <v>133.0</v>
       </c>
       <c s="2" r="F4">
-        <v>844.0</v>
+        <v>491.0</v>
       </c>
       <c s="2" r="G4">
-        <v>657.0</v>
+        <v>286.0</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c s="2" r="B5">
-        <v>628.0</v>
+        <v>1412.0</v>
       </c>
       <c s="2" r="C5">
-        <v>1741.0</v>
+        <v>2249.0</v>
       </c>
       <c s="2" r="D5">
-        <v>1113.0</v>
+        <v>968.0</v>
       </c>
       <c s="2" r="E5">
-        <v>345.0</v>
+        <v>350.0</v>
       </c>
       <c s="2" r="F5">
-        <v>976.0</v>
+        <v>882.0</v>
       </c>
       <c s="2" r="G5">
-        <v>602.0</v>
+        <v>348.0</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c s="2" r="B6">
+        <v>3.0</v>
+      </c>
+      <c s="2" r="C6">
         <v>1.0</v>
-      </c>
-      <c s="2" r="C6">
-        <v>14.0</v>
       </c>
       <c s="2" r="D6">
         <v>2.0</v>
       </c>
       <c s="2" r="E6">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="2" r="F6">
         <v>0.0</v>
@@ -438,77 +811,77 @@
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c s="2" r="B7">
-        <v>12.0</v>
+        <v>16.0</v>
       </c>
       <c s="2" r="C7">
-        <v>35.0</v>
+        <v>36.0</v>
       </c>
       <c s="2" r="D7">
-        <v>36.0</v>
+        <v>11.0</v>
       </c>
       <c s="2" r="E7">
+        <v>0.0</v>
+      </c>
+      <c s="2" r="F7">
         <v>6.0</v>
       </c>
-      <c s="2" r="F7">
-        <v>20.0</v>
-      </c>
       <c s="2" r="G7">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c s="2" r="B8">
-        <v>34.0</v>
+        <v>100.0</v>
       </c>
       <c s="2" r="C8">
-        <v>47.0</v>
+        <v>35.0</v>
       </c>
       <c s="2" r="D8">
-        <v>16.0</v>
+        <v>18.0</v>
       </c>
       <c s="2" r="E8">
-        <v>25.0</v>
+        <v>18.0</v>
       </c>
       <c s="2" r="F8">
-        <v>20.0</v>
+        <v>3.0</v>
       </c>
       <c s="2" r="G8">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c t="str" s="2" r="B9">
         <f ref="B9:G9" t="shared" si="1">sum(B4:B8)</f>
-        <v>1313</v>
+        <v>2249</v>
       </c>
       <c t="str" s="2" r="C9">
         <f t="shared" si="1"/>
-        <v>4089</v>
+        <v>4562</v>
       </c>
       <c t="str" s="2" r="D9">
         <f t="shared" si="1"/>
-        <v>2433</v>
+        <v>2069</v>
       </c>
       <c t="str" s="2" r="E9">
         <f t="shared" si="1"/>
-        <v>673</v>
+        <v>502</v>
       </c>
       <c t="str" s="2" r="F9">
         <f t="shared" si="1"/>
-        <v>1860</v>
+        <v>1382</v>
       </c>
       <c t="str" s="2" r="G9">
         <f t="shared" si="1"/>
-        <v>1270</v>
+        <v>648</v>
       </c>
     </row>
     <row r="10">
@@ -3495,7 +3868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3503,8 +3876,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c t="s" s="3" r="A1">
-        <v>16</v>
+      <c t="s" s="1" r="A1">
+        <v>0</v>
       </c>
       <c s="1" r="H1"/>
       <c s="1" r="I1"/>
@@ -3528,96 +3901,96 @@
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c t="s" s="1" r="E2">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="B3">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c t="s" s="1" r="D3">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c t="s" s="1" r="E3">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c t="s" s="1" r="F3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c t="s" s="1" r="G3">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c s="2" r="B4">
-        <v>718.0</v>
+        <v>638.0</v>
       </c>
       <c s="2" r="C4">
-        <v>2241.0</v>
+        <v>2252.0</v>
       </c>
       <c s="2" r="D4">
-        <v>1070.0</v>
+        <v>1266.0</v>
       </c>
       <c s="2" r="E4">
-        <v>133.0</v>
+        <v>297.0</v>
       </c>
       <c s="2" r="F4">
-        <v>491.0</v>
+        <v>844.0</v>
       </c>
       <c s="2" r="G4">
-        <v>286.0</v>
+        <v>657.0</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c s="2" r="B5">
-        <v>1412.0</v>
+        <v>628.0</v>
       </c>
       <c s="2" r="C5">
-        <v>2249.0</v>
+        <v>1741.0</v>
       </c>
       <c s="2" r="D5">
-        <v>968.0</v>
+        <v>1113.0</v>
       </c>
       <c s="2" r="E5">
-        <v>350.0</v>
+        <v>345.0</v>
       </c>
       <c s="2" r="F5">
-        <v>882.0</v>
+        <v>976.0</v>
       </c>
       <c s="2" r="G5">
-        <v>348.0</v>
+        <v>602.0</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c s="2" r="B6">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c s="2" r="C6">
-        <v>1.0</v>
+        <v>14.0</v>
       </c>
       <c s="2" r="D6">
         <v>2.0</v>
       </c>
       <c s="2" r="E6">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="2" r="F6">
         <v>0.0</v>
@@ -3628,77 +4001,77 @@
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c s="2" r="B7">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c s="2" r="C7">
+        <v>35.0</v>
+      </c>
+      <c s="2" r="D7">
         <v>36.0</v>
       </c>
-      <c s="2" r="D7">
-        <v>11.0</v>
-      </c>
       <c s="2" r="E7">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="F7">
+        <v>20.0</v>
+      </c>
+      <c s="2" r="G7">
         <v>6.0</v>
-      </c>
-      <c s="2" r="G7">
-        <v>8.0</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c s="2" r="B8">
-        <v>100.0</v>
+        <v>34.0</v>
       </c>
       <c s="2" r="C8">
-        <v>35.0</v>
+        <v>47.0</v>
       </c>
       <c s="2" r="D8">
-        <v>18.0</v>
+        <v>16.0</v>
       </c>
       <c s="2" r="E8">
-        <v>18.0</v>
+        <v>25.0</v>
       </c>
       <c s="2" r="F8">
-        <v>3.0</v>
+        <v>20.0</v>
       </c>
       <c s="2" r="G8">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c t="str" s="2" r="B9">
         <f ref="B9:G9" t="shared" si="1">sum(B4:B8)</f>
-        <v>2249</v>
+        <v>1313</v>
       </c>
       <c t="str" s="2" r="C9">
         <f t="shared" si="1"/>
-        <v>4562</v>
+        <v>4089</v>
       </c>
       <c t="str" s="2" r="D9">
         <f t="shared" si="1"/>
-        <v>2069</v>
+        <v>2433</v>
       </c>
       <c t="str" s="2" r="E9">
         <f t="shared" si="1"/>
-        <v>502</v>
+        <v>673</v>
       </c>
       <c t="str" s="2" r="F9">
         <f t="shared" si="1"/>
-        <v>1382</v>
+        <v>1860</v>
       </c>
       <c t="str" s="2" r="G9">
         <f t="shared" si="1"/>
-        <v>648</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="10">
@@ -6685,325 +7058,109 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="53.71"/>
+    <col min="1" customWidth="1" max="1" width="27.86"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c t="s" s="4" r="A1">
-        <v>32</v>
-      </c>
-      <c t="s" s="4" r="B1">
-        <v>33</v>
-      </c>
+      <c t="s" s="1" r="A1">
+        <v>16</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>18</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>19</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>20</v>
+      </c>
+      <c t="s" s="1" r="E1">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="F1">
+        <v>22</v>
+      </c>
+      <c t="s" s="1" r="G1">
+        <v>23</v>
+      </c>
+      <c t="s" s="1" r="H1">
+        <v>24</v>
+      </c>
+      <c t="s" s="1" r="I1">
+        <v>25</v>
+      </c>
+      <c t="s" s="1" r="J1">
+        <v>26</v>
+      </c>
+      <c t="s" s="1" r="K1">
+        <v>27</v>
+      </c>
+      <c t="s" s="1" r="L1">
+        <v>28</v>
+      </c>
+      <c t="s" s="1" r="M1">
+        <v>29</v>
+      </c>
+      <c s="1" r="N1"/>
+      <c s="1" r="O1"/>
+      <c s="1" r="P1"/>
+      <c s="1" r="Q1"/>
+      <c s="1" r="R1"/>
+      <c s="1" r="S1"/>
+      <c s="1" r="T1"/>
+      <c s="1" r="U1"/>
+      <c s="1" r="V1"/>
+      <c s="1" r="W1"/>
+      <c s="1" r="X1"/>
+      <c s="1" r="Y1"/>
+      <c s="1" r="Z1"/>
     </row>
     <row r="2">
       <c t="s" s="4" r="A2">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c s="4" r="B2">
-        <v>509.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c t="s" s="4" r="A3">
-        <v>35</v>
-      </c>
-      <c s="4" r="B3">
-        <v>34.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c t="s" s="4" r="A4">
-        <v>36</v>
-      </c>
-      <c s="4" r="B4">
-        <v>169.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c t="s" s="4" r="A5">
-        <v>37</v>
-      </c>
-      <c s="4" r="B5">
-        <v>261.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="4" r="A6">
-        <v>38</v>
-      </c>
-      <c s="4" r="B6">
-        <v>249.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c t="s" s="4" r="A7">
-        <v>39</v>
-      </c>
-      <c s="4" r="B7">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c t="s" s="4" r="A8">
-        <v>40</v>
-      </c>
-      <c s="4" r="B8">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c t="s" s="4" r="A9">
-        <v>41</v>
-      </c>
-      <c s="4" r="B9">
-        <v>67.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c t="s" s="4" r="A10">
-        <v>42</v>
-      </c>
-      <c s="4" r="B10">
-        <v>29.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c t="s" s="4" r="A11">
-        <v>43</v>
-      </c>
-      <c s="4" r="B11">
-        <v>32.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c t="s" s="4" r="A12">
-        <v>44</v>
-      </c>
-      <c s="4" r="B12">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c t="s" s="4" r="A13">
-        <v>45</v>
-      </c>
-      <c s="4" r="B13">
-        <v>223.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c t="s" s="4" r="A14">
-        <v>46</v>
-      </c>
-      <c s="4" r="B14">
-        <v>473.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c t="s" s="4" r="A15">
-        <v>47</v>
-      </c>
-      <c s="4" r="B15">
-        <v>2862.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c t="s" s="4" r="A16">
-        <v>48</v>
-      </c>
-      <c s="4" r="B16">
-        <v>437.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c t="s" s="4" r="A17">
-        <v>49</v>
-      </c>
-      <c s="4" r="B17">
-        <v>144.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="4" r="A18">
-        <v>50</v>
-      </c>
-      <c s="4" r="B18">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="4" r="A19">
-        <v>51</v>
-      </c>
-      <c s="4" r="B19">
-        <v>1093.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="4" r="A20">
-        <v>52</v>
-      </c>
-      <c s="4" r="B20">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="4" r="A21">
-        <v>53</v>
-      </c>
-      <c s="4" r="B21">
-        <v>32.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c t="s" s="4" r="A22">
-        <v>54</v>
-      </c>
-      <c s="4" r="B22">
-        <v>31.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c t="s" s="4" r="A23">
-        <v>55</v>
-      </c>
-      <c s="4" r="B23">
-        <v>18.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c t="s" s="4" r="A24">
-        <v>56</v>
-      </c>
-      <c s="4" r="B24">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c t="s" s="4" r="A25">
-        <v>57</v>
-      </c>
-      <c s="4" r="B25">
-        <v>1176.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c t="s" s="4" r="A26">
-        <v>58</v>
-      </c>
-      <c s="4" r="B26">
-        <v>3984.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c t="s" s="4" r="A27">
-        <v>59</v>
-      </c>
-      <c s="4" r="B27">
-        <v>2865.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" customWidth="1" max="1" width="35.29"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c t="s" s="4" r="A1">
-        <v>60</v>
-      </c>
-      <c t="s" s="4" r="B1">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2">
-      <c t="s" s="4" r="A2">
-        <v>62</v>
-      </c>
-      <c s="4" r="B2">
-        <v>4378.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c t="s" s="4" r="A3">
-        <v>63</v>
-      </c>
-      <c s="4" r="B3">
-        <v>680.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c t="s" s="4" r="A4">
-        <v>64</v>
-      </c>
-      <c s="4" r="B4">
-        <v>59.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c t="s" s="4" r="A5">
-        <v>65</v>
-      </c>
-      <c s="4" r="B5">
-        <v>43.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="4" r="A6">
-        <v>66</v>
-      </c>
-      <c s="4" r="B6">
-        <v>67.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c t="s" s="4" r="A7">
-        <v>67</v>
-      </c>
-      <c s="4" r="B7">
-        <v>397.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c t="s" s="4" r="A8">
-        <v>68</v>
-      </c>
-      <c s="4" r="B8">
-        <v>108.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c t="s" s="4" r="A9">
-        <v>69</v>
-      </c>
-      <c s="4" r="B9">
-        <v>2328.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c t="s" s="4" r="A10">
-        <v>70</v>
-      </c>
-      <c s="4" r="B10">
-        <v>3701.0</v>
+        <v>828.0</v>
+      </c>
+      <c s="4" r="C2">
+        <v>717.0</v>
+      </c>
+      <c s="4" r="D2">
+        <v>827.0</v>
+      </c>
+      <c s="4" r="E2">
+        <v>881.0</v>
+      </c>
+      <c s="4" r="F2">
+        <v>898.0</v>
+      </c>
+      <c s="4" r="G2">
+        <v>867.0</v>
+      </c>
+      <c s="4" r="H2">
+        <v>939.0</v>
+      </c>
+      <c s="4" r="I2">
+        <v>898.0</v>
+      </c>
+      <c s="4" r="J2">
+        <v>919.0</v>
+      </c>
+      <c s="4" r="K2">
+        <v>896.0</v>
+      </c>
+      <c s="4" r="L2">
+        <v>787.0</v>
+      </c>
+      <c s="4" r="M2">
+        <v>695.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>